<commit_message>
Benchmarked back to v1.1
</commit_message>
<xml_diff>
--- a/datatables/httk-benchmarks.xlsx
+++ b/datatables/httk-benchmarks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwambaug\git\httk-dev\datatables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44566E84-BA42-4EE2-A60E-BBA2BBBDF88B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE5CD292-95AE-4FFD-B34B-043B9068B900}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{C208547E-DF7E-4D1E-AF51-B4A727438EC0}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>2.2.2</t>
   </si>
@@ -121,9 +121,6 @@
     <t>Refactored Monte Carlo functions, likely broke calc_ionization for monte carlo.</t>
   </si>
   <si>
-    <t>Added in vivo data</t>
-  </si>
-  <si>
     <t>calc_mc_css non-functional, NA values replaced with "2"</t>
   </si>
   <si>
@@ -133,15 +130,6 @@
     <t xml:space="preserve">uM units on `calc_mc_css` were incorrectly calculated. Fixed bug that caused ionization to be ignored. Chemicals dropped based on PFC's, volatility. </t>
   </si>
   <si>
-    <t>Too slow</t>
-  </si>
-  <si>
-    <t>Requires argument "method" for calc_mc_css -- need to figure out how to check for that.</t>
-  </si>
-  <si>
-    <t>calc_mc_css does not allow model to be specified</t>
-  </si>
-  <si>
     <t>calc_mc.units</t>
   </si>
   <si>
@@ -149,6 +137,24 @@
   </si>
   <si>
     <t>N.InVivoCss</t>
+  </si>
+  <si>
+    <t>RMSLE.InVivoAUC</t>
+  </si>
+  <si>
+    <t>N.InVivoAUC</t>
+  </si>
+  <si>
+    <t>RMSLE.InVivoCmax</t>
+  </si>
+  <si>
+    <t>N.InVivoCmax</t>
+  </si>
+  <si>
+    <t>Very slow MC sampler</t>
+  </si>
+  <si>
+    <t>HTTK-pop introduced.</t>
   </si>
 </sst>
 </file>
@@ -202,7 +208,19 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="18">
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -431,6 +449,24 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>0.52929999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.52929999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.65449999999999997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.65449999999999997</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.68330000000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.82299999999999995</c:v>
+                </c:pt>
                 <c:pt idx="6">
                   <c:v>0.82299999999999995</c:v>
                 </c:pt>
@@ -994,6 +1030,27 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>1.869</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.869</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.8220000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.8220000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.81</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.9339999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.9339999999999999</c:v>
+                </c:pt>
                 <c:pt idx="7">
                   <c:v>1.8160000000000001</c:v>
                 </c:pt>
@@ -1013,31 +1070,31 @@
                   <c:v>1.873</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.847</c:v>
+                  <c:v>1.89</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.843</c:v>
+                  <c:v>1.9139999999999999</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.843</c:v>
+                  <c:v>1.9139999999999999</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.851</c:v>
+                  <c:v>1.927</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.8520000000000001</c:v>
+                  <c:v>1.7909999999999999</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.857</c:v>
+                  <c:v>1.782</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.7529999999999999</c:v>
+                  <c:v>1.6819999999999999</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1.7529999999999999</c:v>
+                  <c:v>1.6819999999999999</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1.946</c:v>
+                  <c:v>1.9790000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2588,21 +2645,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3DD92D36-BFF3-413F-93A1-8D3D8569B858}" name="Table1" displayName="Table1" ref="A1:L23" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
-  <autoFilter ref="A1:L23" xr:uid="{3DD92D36-BFF3-413F-93A1-8D3D8569B858}"/>
-  <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{478C9B49-D67B-44BA-B8BF-86E093E572FE}" name="Version" dataDxfId="11"/>
-    <tableColumn id="13" xr3:uid="{1CCFB984-6FEC-43E4-BB73-000E230E2655}" name="N.steadystate" dataDxfId="10"/>
-    <tableColumn id="12" xr3:uid="{A3AE1B91-13E0-467A-B253-DD55F1CDDDC8}" name="calc_analytic.units" dataDxfId="9"/>
-    <tableColumn id="11" xr3:uid="{A1A34259-FB8E-4CB8-96E2-4F0D0A685508}" name="calc_mc.units" dataDxfId="8"/>
-    <tableColumn id="10" xr3:uid="{B2CEC2E9-5F34-4C70-ACC0-64C0D9276426}" name="solve_pbtk.units" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{0EAB2FF6-C940-45E5-AA07-66498BE7AE45}" name="RMSLE.Wetmore" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{74DF6239-A9CF-4285-93A5-E0836BE33ED4}" name="N.Wetmore" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{32F7A55C-552D-4FE2-A1C9-DDE5CE343E38}" name="RMSLE.noMC" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{EE86B53C-98F4-4257-9A15-953203686624}" name="N.noMC" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{44929D55-8AA6-4725-BA9A-148E5B9C389A}" name="RMSLE.InVivoCss" dataDxfId="2"/>
-    <tableColumn id="14" xr3:uid="{1AADC521-88C8-4578-A079-64B13EC6DCF7}" name="N.InVivoCss" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{77576EAB-F3B7-477C-9C89-32194666C30A}" name="Notes" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3DD92D36-BFF3-413F-93A1-8D3D8569B858}" name="Table1" displayName="Table1" ref="A1:P23" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+  <autoFilter ref="A1:P23" xr:uid="{3DD92D36-BFF3-413F-93A1-8D3D8569B858}"/>
+  <tableColumns count="16">
+    <tableColumn id="1" xr3:uid="{478C9B49-D67B-44BA-B8BF-86E093E572FE}" name="Version" dataDxfId="15"/>
+    <tableColumn id="13" xr3:uid="{1CCFB984-6FEC-43E4-BB73-000E230E2655}" name="N.steadystate" dataDxfId="14"/>
+    <tableColumn id="12" xr3:uid="{A3AE1B91-13E0-467A-B253-DD55F1CDDDC8}" name="calc_analytic.units" dataDxfId="13"/>
+    <tableColumn id="11" xr3:uid="{A1A34259-FB8E-4CB8-96E2-4F0D0A685508}" name="calc_mc.units" dataDxfId="12"/>
+    <tableColumn id="10" xr3:uid="{B2CEC2E9-5F34-4C70-ACC0-64C0D9276426}" name="solve_pbtk.units" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{0EAB2FF6-C940-45E5-AA07-66498BE7AE45}" name="RMSLE.Wetmore" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{74DF6239-A9CF-4285-93A5-E0836BE33ED4}" name="N.Wetmore" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{32F7A55C-552D-4FE2-A1C9-DDE5CE343E38}" name="RMSLE.noMC" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{EE86B53C-98F4-4257-9A15-953203686624}" name="N.noMC" dataDxfId="7"/>
+    <tableColumn id="8" xr3:uid="{44929D55-8AA6-4725-BA9A-148E5B9C389A}" name="RMSLE.InVivoCss" dataDxfId="6"/>
+    <tableColumn id="14" xr3:uid="{1AADC521-88C8-4578-A079-64B13EC6DCF7}" name="N.InVivoCss" dataDxfId="5"/>
+    <tableColumn id="16" xr3:uid="{94142C49-62AE-4C38-93E2-90BE502E5B9F}" name="RMSLE.InVivoAUC" dataDxfId="0"/>
+    <tableColumn id="15" xr3:uid="{42F79D9D-6A9A-4290-976D-8FC7D0C64550}" name="N.InVivoAUC" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{26964959-0CEF-47FA-B3F1-3787B56AAF4B}" name="RMSLE.InVivoCmax" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{C36A3E11-DF44-49AF-81EC-5DDE1C9E24BF}" name="N.InVivoCmax" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{77576EAB-F3B7-477C-9C89-32194666C30A}" name="Notes" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2905,10 +2966,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AA7C988-D5EA-4528-8554-7DA2671EBD43}">
-  <dimension ref="A1:L23"/>
+  <dimension ref="A1:P23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2918,11 +2979,11 @@
     <col min="7" max="7" width="12.81640625" customWidth="1"/>
     <col min="8" max="8" width="13.81640625" customWidth="1"/>
     <col min="9" max="10" width="9.7265625" customWidth="1"/>
-    <col min="11" max="11" width="6.54296875" customWidth="1"/>
-    <col min="12" max="12" width="39.453125" customWidth="1"/>
+    <col min="11" max="15" width="6.7265625" customWidth="1"/>
+    <col min="16" max="16" width="39.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -2933,7 +2994,7 @@
         <v>23</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>24</v>
@@ -2951,118 +3012,320 @@
         <v>6</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
+      <c r="B2" s="1">
+        <v>349</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0.52929999999999999</v>
+      </c>
+      <c r="G2" s="1">
+        <v>237</v>
+      </c>
+      <c r="H2" s="1">
+        <v>0.10929999999999999</v>
+      </c>
+      <c r="I2" s="1">
+        <v>237</v>
+      </c>
+      <c r="J2" s="1">
+        <v>1.869</v>
+      </c>
+      <c r="K2" s="1">
+        <v>30</v>
+      </c>
+      <c r="L2" s="1">
+        <v>0.96870000000000001</v>
+      </c>
+      <c r="M2" s="1">
+        <v>53</v>
+      </c>
+      <c r="N2" s="1">
+        <v>1.5589999999999999</v>
+      </c>
+      <c r="O2" s="1">
+        <v>53</v>
+      </c>
+      <c r="P2" s="1"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1.2</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
+      <c r="B3" s="1">
+        <v>349</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0.52929999999999999</v>
+      </c>
+      <c r="G3" s="1">
+        <v>237</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0.10929999999999999</v>
+      </c>
+      <c r="I3" s="1">
+        <v>237</v>
+      </c>
+      <c r="J3" s="1">
+        <v>1.869</v>
+      </c>
+      <c r="K3" s="1">
+        <v>30</v>
+      </c>
+      <c r="L3" s="1">
+        <v>1.107</v>
+      </c>
+      <c r="M3" s="1">
+        <v>83</v>
+      </c>
+      <c r="N3" s="1">
+        <v>1.4370000000000001</v>
+      </c>
+      <c r="O3" s="1">
+        <v>83</v>
+      </c>
+      <c r="P3" s="1"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>1.3</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
+      <c r="B4" s="1">
+        <v>543</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0.65449999999999997</v>
+      </c>
+      <c r="G4" s="1">
+        <v>398</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0.12570000000000001</v>
+      </c>
+      <c r="I4" s="1">
+        <v>398</v>
+      </c>
+      <c r="J4" s="1">
+        <v>1.8220000000000001</v>
+      </c>
+      <c r="K4" s="1">
+        <v>31</v>
+      </c>
+      <c r="L4" s="1">
+        <v>1.0940000000000001</v>
+      </c>
+      <c r="M4" s="1">
+        <v>89</v>
+      </c>
+      <c r="N4" s="1">
+        <v>1.413</v>
+      </c>
+      <c r="O4" s="1">
+        <v>89</v>
+      </c>
+      <c r="P4" s="1"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>1.4</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1" t="s">
-        <v>33</v>
-      </c>
+      <c r="B5" s="1">
+        <v>543</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0.65449999999999997</v>
+      </c>
+      <c r="G5" s="1">
+        <v>398</v>
+      </c>
+      <c r="H5" s="1">
+        <v>0.12570000000000001</v>
+      </c>
+      <c r="I5" s="1">
+        <v>398</v>
+      </c>
+      <c r="J5" s="1">
+        <v>1.8220000000000001</v>
+      </c>
+      <c r="K5" s="1">
+        <v>31</v>
+      </c>
+      <c r="L5" s="1">
+        <v>1.0940000000000001</v>
+      </c>
+      <c r="M5" s="1">
+        <v>89</v>
+      </c>
+      <c r="N5" s="1">
+        <v>1.413</v>
+      </c>
+      <c r="O5" s="1">
+        <v>89</v>
+      </c>
+      <c r="P5" s="1"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>1.5</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1" t="s">
-        <v>32</v>
+      <c r="B6" s="1">
+        <v>543</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1">
+        <v>1</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0.68330000000000002</v>
+      </c>
+      <c r="G6" s="1">
+        <v>398</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="I6" s="1">
+        <v>398</v>
+      </c>
+      <c r="J6" s="1">
+        <v>1.81</v>
+      </c>
+      <c r="K6" s="1">
+        <v>31</v>
+      </c>
+      <c r="L6" s="1">
+        <v>1.093</v>
+      </c>
+      <c r="M6" s="1">
+        <v>87</v>
+      </c>
+      <c r="N6" s="1">
+        <v>1.4059999999999999</v>
+      </c>
+      <c r="O6" s="1">
+        <v>87</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>1.6</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1" t="s">
+      <c r="B7" s="1">
+        <v>553</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1">
+        <v>1</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0.82299999999999995</v>
+      </c>
+      <c r="G7" s="1">
+        <v>397</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0.45950000000000002</v>
+      </c>
+      <c r="I7" s="1">
+        <v>397</v>
+      </c>
+      <c r="J7" s="1">
+        <v>1.9339999999999999</v>
+      </c>
+      <c r="K7" s="1">
         <v>31</v>
       </c>
+      <c r="L7" s="1">
+        <v>1.33</v>
+      </c>
+      <c r="M7" s="1">
+        <v>87</v>
+      </c>
+      <c r="N7" s="1">
+        <v>1.7110000000000001</v>
+      </c>
+      <c r="O7" s="1">
+        <v>87</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>1.7</v>
       </c>
@@ -3090,11 +3353,27 @@
       <c r="I8" s="1">
         <v>397</v>
       </c>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
+      <c r="J8" s="1">
+        <v>1.9339999999999999</v>
+      </c>
+      <c r="K8" s="1">
+        <v>31</v>
+      </c>
+      <c r="L8" s="1">
+        <v>1.33</v>
+      </c>
+      <c r="M8" s="1">
+        <v>87</v>
+      </c>
+      <c r="N8" s="1">
+        <v>1.7110000000000001</v>
+      </c>
+      <c r="O8" s="1">
+        <v>87</v>
+      </c>
+      <c r="P8" s="1"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>1.8</v>
       </c>
@@ -3128,11 +3407,21 @@
       <c r="K9" s="1">
         <v>33</v>
       </c>
-      <c r="L9" s="1" t="s">
-        <v>27</v>
-      </c>
+      <c r="L9" s="1">
+        <v>1.327</v>
+      </c>
+      <c r="M9" s="1">
+        <v>89</v>
+      </c>
+      <c r="N9" s="1">
+        <v>1.7230000000000001</v>
+      </c>
+      <c r="O9" s="1">
+        <v>89</v>
+      </c>
+      <c r="P9" s="1"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>1.9</v>
       </c>
@@ -3166,9 +3455,21 @@
       <c r="K10" s="1">
         <v>31</v>
       </c>
-      <c r="L10" s="1"/>
+      <c r="L10" s="1">
+        <v>1.274</v>
+      </c>
+      <c r="M10" s="1">
+        <v>89</v>
+      </c>
+      <c r="N10" s="1">
+        <v>1.6970000000000001</v>
+      </c>
+      <c r="O10" s="1">
+        <v>89</v>
+      </c>
+      <c r="P10" s="1"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
@@ -3202,11 +3503,23 @@
       <c r="K11" s="1">
         <v>31</v>
       </c>
-      <c r="L11" s="1" t="s">
-        <v>28</v>
+      <c r="L11" s="1">
+        <v>1.274</v>
+      </c>
+      <c r="M11" s="1">
+        <v>89</v>
+      </c>
+      <c r="N11" s="1">
+        <v>1.6970000000000001</v>
+      </c>
+      <c r="O11" s="1">
+        <v>89</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>4</v>
       </c>
@@ -3240,9 +3553,21 @@
       <c r="K12" s="1">
         <v>31</v>
       </c>
-      <c r="L12" s="1"/>
+      <c r="L12" s="1">
+        <v>1.274</v>
+      </c>
+      <c r="M12" s="1">
+        <v>89</v>
+      </c>
+      <c r="N12" s="1">
+        <v>1.6970000000000001</v>
+      </c>
+      <c r="O12" s="1">
+        <v>89</v>
+      </c>
+      <c r="P12" s="1"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
@@ -3276,11 +3601,23 @@
       <c r="K13" s="1">
         <v>31</v>
       </c>
-      <c r="L13" s="1" t="s">
+      <c r="L13" s="1">
+        <v>1.284</v>
+      </c>
+      <c r="M13" s="1">
+        <v>85</v>
+      </c>
+      <c r="N13" s="1">
+        <v>1.7</v>
+      </c>
+      <c r="O13" s="1">
+        <v>85</v>
+      </c>
+      <c r="P13" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>17</v>
       </c>
@@ -3314,9 +3651,21 @@
       <c r="K14" s="1">
         <v>31</v>
       </c>
-      <c r="L14" s="1"/>
+      <c r="L14" s="1">
+        <v>1.284</v>
+      </c>
+      <c r="M14" s="1">
+        <v>85</v>
+      </c>
+      <c r="N14" s="1">
+        <v>1.7</v>
+      </c>
+      <c r="O14" s="1">
+        <v>85</v>
+      </c>
+      <c r="P14" s="1"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>7</v>
       </c>
@@ -3345,16 +3694,28 @@
         <v>397</v>
       </c>
       <c r="J15" s="1">
-        <v>1.847</v>
+        <v>1.89</v>
       </c>
       <c r="K15" s="1">
-        <v>28</v>
-      </c>
-      <c r="L15" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L15" s="1">
+        <v>1.278</v>
+      </c>
+      <c r="M15" s="1">
+        <v>83</v>
+      </c>
+      <c r="N15" s="1">
+        <v>1.179</v>
+      </c>
+      <c r="O15" s="1">
+        <v>83</v>
+      </c>
+      <c r="P15" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -3383,14 +3744,26 @@
         <v>401</v>
       </c>
       <c r="J16" s="1">
-        <v>1.843</v>
+        <v>1.9139999999999999</v>
       </c>
       <c r="K16" s="1">
-        <v>28</v>
-      </c>
-      <c r="L16" s="1"/>
+        <v>31</v>
+      </c>
+      <c r="L16" s="1">
+        <v>1.2769999999999999</v>
+      </c>
+      <c r="M16" s="1">
+        <v>83</v>
+      </c>
+      <c r="N16" s="1">
+        <v>1.1879999999999999</v>
+      </c>
+      <c r="O16" s="1">
+        <v>83</v>
+      </c>
+      <c r="P16" s="1"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>13</v>
       </c>
@@ -3419,14 +3792,26 @@
         <v>401</v>
       </c>
       <c r="J17" s="1">
-        <v>1.843</v>
+        <v>1.9139999999999999</v>
       </c>
       <c r="K17" s="1">
-        <v>28</v>
-      </c>
-      <c r="L17" s="1"/>
+        <v>31</v>
+      </c>
+      <c r="L17" s="1">
+        <v>1.2769999999999999</v>
+      </c>
+      <c r="M17" s="1">
+        <v>83</v>
+      </c>
+      <c r="N17" s="1">
+        <v>1.1879999999999999</v>
+      </c>
+      <c r="O17" s="1">
+        <v>83</v>
+      </c>
+      <c r="P17" s="1"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>12</v>
       </c>
@@ -3455,14 +3840,26 @@
         <v>401</v>
       </c>
       <c r="J18" s="1">
-        <v>1.851</v>
+        <v>1.927</v>
       </c>
       <c r="K18" s="1">
-        <v>28</v>
-      </c>
-      <c r="L18" s="1"/>
+        <v>31</v>
+      </c>
+      <c r="L18" s="1">
+        <v>1.3360000000000001</v>
+      </c>
+      <c r="M18" s="1">
+        <v>90</v>
+      </c>
+      <c r="N18" s="1">
+        <v>1.2450000000000001</v>
+      </c>
+      <c r="O18" s="1">
+        <v>90</v>
+      </c>
+      <c r="P18" s="1"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>11</v>
       </c>
@@ -3491,14 +3888,26 @@
         <v>398</v>
       </c>
       <c r="J19" s="1">
-        <v>1.8520000000000001</v>
+        <v>1.7909999999999999</v>
       </c>
       <c r="K19" s="1">
-        <v>28</v>
-      </c>
-      <c r="L19" s="1"/>
+        <v>31</v>
+      </c>
+      <c r="L19" s="1">
+        <v>1.28</v>
+      </c>
+      <c r="M19" s="1">
+        <v>90</v>
+      </c>
+      <c r="N19" s="1">
+        <v>1.228</v>
+      </c>
+      <c r="O19" s="1">
+        <v>90</v>
+      </c>
+      <c r="P19" s="1"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>10</v>
       </c>
@@ -3527,16 +3936,28 @@
         <v>371</v>
       </c>
       <c r="J20" s="1">
-        <v>1.857</v>
+        <v>1.782</v>
       </c>
       <c r="K20" s="1">
-        <v>28</v>
-      </c>
-      <c r="L20" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
+      </c>
+      <c r="L20" s="1">
+        <v>1.274</v>
+      </c>
+      <c r="M20" s="1">
+        <v>88</v>
+      </c>
+      <c r="N20" s="1">
+        <v>1.21</v>
+      </c>
+      <c r="O20" s="1">
+        <v>88</v>
+      </c>
+      <c r="P20" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>9</v>
       </c>
@@ -3565,16 +3986,28 @@
         <v>370</v>
       </c>
       <c r="J21" s="1">
-        <v>1.7529999999999999</v>
+        <v>1.6819999999999999</v>
       </c>
       <c r="K21" s="1">
-        <v>28</v>
-      </c>
-      <c r="L21" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L21" s="1">
+        <v>1.1619999999999999</v>
+      </c>
+      <c r="M21" s="1">
+        <v>88</v>
+      </c>
+      <c r="N21" s="1">
+        <v>1.1180000000000001</v>
+      </c>
+      <c r="O21" s="1">
+        <v>88</v>
+      </c>
+      <c r="P21" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>3</v>
       </c>
@@ -3603,14 +4036,26 @@
         <v>370</v>
       </c>
       <c r="J22" s="1">
-        <v>1.7529999999999999</v>
+        <v>1.6819999999999999</v>
       </c>
       <c r="K22" s="1">
-        <v>28</v>
-      </c>
-      <c r="L22" s="1"/>
+        <v>31</v>
+      </c>
+      <c r="L22" s="1">
+        <v>1.1619999999999999</v>
+      </c>
+      <c r="M22" s="1">
+        <v>88</v>
+      </c>
+      <c r="N22" s="1">
+        <v>1.1180000000000001</v>
+      </c>
+      <c r="O22" s="1">
+        <v>88</v>
+      </c>
+      <c r="P22" s="1"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>0</v>
       </c>
@@ -3639,13 +4084,25 @@
         <v>370</v>
       </c>
       <c r="J23" s="1">
-        <v>1.946</v>
+        <v>1.9790000000000001</v>
       </c>
       <c r="K23" s="1">
+        <v>31</v>
+      </c>
+      <c r="L23" s="1">
+        <v>1.379</v>
+      </c>
+      <c r="M23" s="1">
+        <v>88</v>
+      </c>
+      <c r="N23" s="1">
+        <v>1.248</v>
+      </c>
+      <c r="O23" s="1">
+        <v>88</v>
+      </c>
+      <c r="P23" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="L23" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Tissue PC test to benchmarks
</commit_message>
<xml_diff>
--- a/datatables/httk-benchmarks.xlsx
+++ b/datatables/httk-benchmarks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwambaug\git\httk-dev\datatables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE5CD292-95AE-4FFD-B34B-043B9068B900}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{975D5C30-FFEA-4D5E-AC8B-50CAF47429DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{C208547E-DF7E-4D1E-AF51-B4A727438EC0}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>2.2.2</t>
   </si>
@@ -156,6 +156,12 @@
   <si>
     <t>HTTK-pop introduced.</t>
   </si>
+  <si>
+    <t>RMSLE.TissuePC</t>
+  </si>
+  <si>
+    <t>N.TissuePC</t>
+  </si>
 </sst>
 </file>
 
@@ -208,7 +214,13 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="20">
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -2645,25 +2657,27 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3DD92D36-BFF3-413F-93A1-8D3D8569B858}" name="Table1" displayName="Table1" ref="A1:P23" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
-  <autoFilter ref="A1:P23" xr:uid="{3DD92D36-BFF3-413F-93A1-8D3D8569B858}"/>
-  <tableColumns count="16">
-    <tableColumn id="1" xr3:uid="{478C9B49-D67B-44BA-B8BF-86E093E572FE}" name="Version" dataDxfId="15"/>
-    <tableColumn id="13" xr3:uid="{1CCFB984-6FEC-43E4-BB73-000E230E2655}" name="N.steadystate" dataDxfId="14"/>
-    <tableColumn id="12" xr3:uid="{A3AE1B91-13E0-467A-B253-DD55F1CDDDC8}" name="calc_analytic.units" dataDxfId="13"/>
-    <tableColumn id="11" xr3:uid="{A1A34259-FB8E-4CB8-96E2-4F0D0A685508}" name="calc_mc.units" dataDxfId="12"/>
-    <tableColumn id="10" xr3:uid="{B2CEC2E9-5F34-4C70-ACC0-64C0D9276426}" name="solve_pbtk.units" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{0EAB2FF6-C940-45E5-AA07-66498BE7AE45}" name="RMSLE.Wetmore" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{74DF6239-A9CF-4285-93A5-E0836BE33ED4}" name="N.Wetmore" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{32F7A55C-552D-4FE2-A1C9-DDE5CE343E38}" name="RMSLE.noMC" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{EE86B53C-98F4-4257-9A15-953203686624}" name="N.noMC" dataDxfId="7"/>
-    <tableColumn id="8" xr3:uid="{44929D55-8AA6-4725-BA9A-148E5B9C389A}" name="RMSLE.InVivoCss" dataDxfId="6"/>
-    <tableColumn id="14" xr3:uid="{1AADC521-88C8-4578-A079-64B13EC6DCF7}" name="N.InVivoCss" dataDxfId="5"/>
-    <tableColumn id="16" xr3:uid="{94142C49-62AE-4C38-93E2-90BE502E5B9F}" name="RMSLE.InVivoAUC" dataDxfId="0"/>
-    <tableColumn id="15" xr3:uid="{42F79D9D-6A9A-4290-976D-8FC7D0C64550}" name="N.InVivoAUC" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{26964959-0CEF-47FA-B3F1-3787B56AAF4B}" name="RMSLE.InVivoCmax" dataDxfId="2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3DD92D36-BFF3-413F-93A1-8D3D8569B858}" name="Table1" displayName="Table1" ref="A1:R23" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
+  <autoFilter ref="A1:R23" xr:uid="{3DD92D36-BFF3-413F-93A1-8D3D8569B858}"/>
+  <tableColumns count="18">
+    <tableColumn id="1" xr3:uid="{478C9B49-D67B-44BA-B8BF-86E093E572FE}" name="Version" dataDxfId="17"/>
+    <tableColumn id="13" xr3:uid="{1CCFB984-6FEC-43E4-BB73-000E230E2655}" name="N.steadystate" dataDxfId="16"/>
+    <tableColumn id="12" xr3:uid="{A3AE1B91-13E0-467A-B253-DD55F1CDDDC8}" name="calc_analytic.units" dataDxfId="15"/>
+    <tableColumn id="11" xr3:uid="{A1A34259-FB8E-4CB8-96E2-4F0D0A685508}" name="calc_mc.units" dataDxfId="14"/>
+    <tableColumn id="10" xr3:uid="{B2CEC2E9-5F34-4C70-ACC0-64C0D9276426}" name="solve_pbtk.units" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{0EAB2FF6-C940-45E5-AA07-66498BE7AE45}" name="RMSLE.Wetmore" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{74DF6239-A9CF-4285-93A5-E0836BE33ED4}" name="N.Wetmore" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{32F7A55C-552D-4FE2-A1C9-DDE5CE343E38}" name="RMSLE.noMC" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{EE86B53C-98F4-4257-9A15-953203686624}" name="N.noMC" dataDxfId="9"/>
+    <tableColumn id="8" xr3:uid="{44929D55-8AA6-4725-BA9A-148E5B9C389A}" name="RMSLE.InVivoCss" dataDxfId="8"/>
+    <tableColumn id="14" xr3:uid="{1AADC521-88C8-4578-A079-64B13EC6DCF7}" name="N.InVivoCss" dataDxfId="7"/>
+    <tableColumn id="16" xr3:uid="{94142C49-62AE-4C38-93E2-90BE502E5B9F}" name="RMSLE.InVivoAUC" dataDxfId="6"/>
+    <tableColumn id="15" xr3:uid="{42F79D9D-6A9A-4290-976D-8FC7D0C64550}" name="N.InVivoAUC" dataDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{26964959-0CEF-47FA-B3F1-3787B56AAF4B}" name="RMSLE.InVivoCmax" dataDxfId="4"/>
     <tableColumn id="7" xr3:uid="{C36A3E11-DF44-49AF-81EC-5DDE1C9E24BF}" name="N.InVivoCmax" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{77576EAB-F3B7-477C-9C89-32194666C30A}" name="Notes" dataDxfId="4"/>
+    <tableColumn id="18" xr3:uid="{DE399DF2-3D30-49D7-8319-CE0FA08C654A}" name="RMSLE.TissuePC" dataDxfId="0"/>
+    <tableColumn id="17" xr3:uid="{823AC9A4-09B8-47F3-A4C2-9EBE5D82251D}" name="N.TissuePC" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{77576EAB-F3B7-477C-9C89-32194666C30A}" name="Notes" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2966,10 +2980,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AA7C988-D5EA-4528-8554-7DA2671EBD43}">
-  <dimension ref="A1:P23"/>
+  <dimension ref="A1:R23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="R4" sqref="R4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2979,11 +2993,11 @@
     <col min="7" max="7" width="12.81640625" customWidth="1"/>
     <col min="8" max="8" width="13.81640625" customWidth="1"/>
     <col min="9" max="10" width="9.7265625" customWidth="1"/>
-    <col min="11" max="15" width="6.7265625" customWidth="1"/>
-    <col min="16" max="16" width="39.453125" customWidth="1"/>
+    <col min="11" max="17" width="6.7265625" customWidth="1"/>
+    <col min="18" max="18" width="39.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -3030,10 +3044,16 @@
         <v>36</v>
       </c>
       <c r="P1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>1.1000000000000001</v>
       </c>
@@ -3080,8 +3100,10 @@
         <v>53</v>
       </c>
       <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1.2</v>
       </c>
@@ -3128,8 +3150,10 @@
         <v>83</v>
       </c>
       <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>1.3</v>
       </c>
@@ -3175,9 +3199,15 @@
       <c r="O4" s="1">
         <v>89</v>
       </c>
-      <c r="P4" s="1"/>
+      <c r="P4" s="1">
+        <v>0.4612</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>12</v>
+      </c>
+      <c r="R4" s="1"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>1.4</v>
       </c>
@@ -3223,9 +3253,15 @@
       <c r="O5" s="1">
         <v>89</v>
       </c>
-      <c r="P5" s="1"/>
+      <c r="P5" s="1">
+        <v>0.4612</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>12</v>
+      </c>
+      <c r="R5" s="1"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>1.5</v>
       </c>
@@ -3271,11 +3307,17 @@
       <c r="O6" s="1">
         <v>87</v>
       </c>
-      <c r="P6" s="1" t="s">
+      <c r="P6" s="1">
+        <v>0.55630000000000002</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>412</v>
+      </c>
+      <c r="R6" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>1.6</v>
       </c>
@@ -3321,11 +3363,17 @@
       <c r="O7" s="1">
         <v>87</v>
       </c>
-      <c r="P7" s="1" t="s">
+      <c r="P7" s="1">
+        <v>0.59250000000000003</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>964</v>
+      </c>
+      <c r="R7" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>1.7</v>
       </c>
@@ -3371,9 +3419,15 @@
       <c r="O8" s="1">
         <v>87</v>
       </c>
-      <c r="P8" s="1"/>
+      <c r="P8" s="1">
+        <v>0.59260000000000002</v>
+      </c>
+      <c r="Q8" s="1">
+        <v>964</v>
+      </c>
+      <c r="R8" s="1"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>1.8</v>
       </c>
@@ -3419,9 +3473,15 @@
       <c r="O9" s="1">
         <v>89</v>
       </c>
-      <c r="P9" s="1"/>
+      <c r="P9" s="1">
+        <v>0.59250000000000003</v>
+      </c>
+      <c r="Q9" s="1">
+        <v>964</v>
+      </c>
+      <c r="R9" s="1"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>1.9</v>
       </c>
@@ -3467,9 +3527,15 @@
       <c r="O10" s="1">
         <v>89</v>
       </c>
-      <c r="P10" s="1"/>
+      <c r="P10" s="1">
+        <v>0.61360000000000003</v>
+      </c>
+      <c r="Q10" s="1">
+        <v>953</v>
+      </c>
+      <c r="R10" s="1"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
@@ -3515,11 +3581,17 @@
       <c r="O11" s="1">
         <v>89</v>
       </c>
-      <c r="P11" s="1" t="s">
+      <c r="P11" s="1">
+        <v>0.61360000000000003</v>
+      </c>
+      <c r="Q11" s="1">
+        <v>953</v>
+      </c>
+      <c r="R11" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>4</v>
       </c>
@@ -3565,9 +3637,15 @@
       <c r="O12" s="1">
         <v>89</v>
       </c>
-      <c r="P12" s="1"/>
+      <c r="P12" s="1">
+        <v>0.61360000000000003</v>
+      </c>
+      <c r="Q12" s="1">
+        <v>953</v>
+      </c>
+      <c r="R12" s="1"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
@@ -3613,11 +3691,17 @@
       <c r="O13" s="1">
         <v>85</v>
       </c>
-      <c r="P13" s="1" t="s">
+      <c r="P13" s="1">
+        <v>0.61150000000000004</v>
+      </c>
+      <c r="Q13" s="1">
+        <v>964</v>
+      </c>
+      <c r="R13" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>17</v>
       </c>
@@ -3663,9 +3747,15 @@
       <c r="O14" s="1">
         <v>85</v>
       </c>
-      <c r="P14" s="1"/>
+      <c r="P14" s="1">
+        <v>0.61150000000000004</v>
+      </c>
+      <c r="Q14" s="1">
+        <v>964</v>
+      </c>
+      <c r="R14" s="1"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>7</v>
       </c>
@@ -3711,11 +3801,17 @@
       <c r="O15" s="1">
         <v>83</v>
       </c>
-      <c r="P15" s="1" t="s">
+      <c r="P15" s="1">
+        <v>0.60980000000000001</v>
+      </c>
+      <c r="Q15" s="1">
+        <v>858</v>
+      </c>
+      <c r="R15" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -3761,9 +3857,15 @@
       <c r="O16" s="1">
         <v>83</v>
       </c>
-      <c r="P16" s="1"/>
+      <c r="P16" s="1">
+        <v>0.7611</v>
+      </c>
+      <c r="Q16" s="1">
+        <v>858</v>
+      </c>
+      <c r="R16" s="1"/>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>13</v>
       </c>
@@ -3809,9 +3911,15 @@
       <c r="O17" s="1">
         <v>83</v>
       </c>
-      <c r="P17" s="1"/>
+      <c r="P17" s="1">
+        <v>0.7611</v>
+      </c>
+      <c r="Q17" s="1">
+        <v>858</v>
+      </c>
+      <c r="R17" s="1"/>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>12</v>
       </c>
@@ -3857,9 +3965,15 @@
       <c r="O18" s="1">
         <v>90</v>
       </c>
-      <c r="P18" s="1"/>
+      <c r="P18" s="1">
+        <v>0.78539999999999999</v>
+      </c>
+      <c r="Q18" s="1">
+        <v>851</v>
+      </c>
+      <c r="R18" s="1"/>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>11</v>
       </c>
@@ -3905,9 +4019,15 @@
       <c r="O19" s="1">
         <v>90</v>
       </c>
-      <c r="P19" s="1"/>
+      <c r="P19" s="1">
+        <v>0.78659999999999997</v>
+      </c>
+      <c r="Q19" s="1">
+        <v>840</v>
+      </c>
+      <c r="R19" s="1"/>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>10</v>
       </c>
@@ -3953,11 +4073,17 @@
       <c r="O20" s="1">
         <v>88</v>
       </c>
-      <c r="P20" s="1" t="s">
+      <c r="P20" s="1">
+        <v>0.59950000000000003</v>
+      </c>
+      <c r="Q20" s="1">
+        <v>863</v>
+      </c>
+      <c r="R20" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>9</v>
       </c>
@@ -4003,11 +4129,17 @@
       <c r="O21" s="1">
         <v>88</v>
       </c>
-      <c r="P21" s="1" t="s">
+      <c r="P21" s="1">
+        <v>0.64280000000000004</v>
+      </c>
+      <c r="Q21" s="1">
+        <v>863</v>
+      </c>
+      <c r="R21" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>3</v>
       </c>
@@ -4053,9 +4185,15 @@
       <c r="O22" s="1">
         <v>88</v>
       </c>
-      <c r="P22" s="1"/>
+      <c r="P22" s="1">
+        <v>0.64300000000000002</v>
+      </c>
+      <c r="Q22" s="1">
+        <v>863</v>
+      </c>
+      <c r="R22" s="1"/>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>0</v>
       </c>
@@ -4101,7 +4239,13 @@
       <c r="O23" s="1">
         <v>88</v>
       </c>
-      <c r="P23" s="1" t="s">
+      <c r="P23" s="1">
+        <v>0.63</v>
+      </c>
+      <c r="Q23" s="1">
+        <v>863</v>
+      </c>
+      <c r="R23" s="1" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added invivoPKfit outputs to dashboard script
</commit_message>
<xml_diff>
--- a/datatables/httk-benchmarks.xlsx
+++ b/datatables/httk-benchmarks.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwambaug\git\httk-dev\datatables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{975D5C30-FFEA-4D5E-AC8B-50CAF47429DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF2A6746-B4AF-4CCF-96A2-50EBF81CE3B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{C208547E-DF7E-4D1E-AF51-B4A727438EC0}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>2.2.2</t>
   </si>
@@ -161,6 +161,12 @@
   </si>
   <si>
     <t>N.TissuePC</t>
+  </si>
+  <si>
+    <t>2.3.0</t>
+  </si>
+  <si>
+    <t>Used Caco-2 to replace Fabs=Fgut=1</t>
   </si>
 </sst>
 </file>
@@ -383,9 +389,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$23</c:f>
+              <c:f>Sheet1!$A$2:$A$24</c:f>
               <c:strCache>
-                <c:ptCount val="22"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>1.1</c:v>
                 </c:pt>
@@ -451,16 +457,19 @@
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>2.2.2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.3.0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$2:$F$23</c:f>
+              <c:f>Sheet1!$F$2:$F$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>0.52929999999999999</c:v>
                 </c:pt>
@@ -526,6 +535,9 @@
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>1.087</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.0629999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -964,9 +976,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$23</c:f>
+              <c:f>Sheet1!$A$2:$A$24</c:f>
               <c:strCache>
-                <c:ptCount val="22"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>1.1</c:v>
                 </c:pt>
@@ -1032,16 +1044,19 @@
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>2.2.2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.3.0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$J$2:$J$23</c:f>
+              <c:f>Sheet1!$J$2:$J$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>1.869</c:v>
                 </c:pt>
@@ -1107,6 +1122,9 @@
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>1.9790000000000001</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.419</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2657,8 +2675,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3DD92D36-BFF3-413F-93A1-8D3D8569B858}" name="Table1" displayName="Table1" ref="A1:R23" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
-  <autoFilter ref="A1:R23" xr:uid="{3DD92D36-BFF3-413F-93A1-8D3D8569B858}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3DD92D36-BFF3-413F-93A1-8D3D8569B858}" name="Table1" displayName="Table1" ref="A1:R24" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
+  <autoFilter ref="A1:R24" xr:uid="{3DD92D36-BFF3-413F-93A1-8D3D8569B858}"/>
   <tableColumns count="18">
     <tableColumn id="1" xr3:uid="{478C9B49-D67B-44BA-B8BF-86E093E572FE}" name="Version" dataDxfId="17"/>
     <tableColumn id="13" xr3:uid="{1CCFB984-6FEC-43E4-BB73-000E230E2655}" name="N.steadystate" dataDxfId="16"/>
@@ -2675,9 +2693,9 @@
     <tableColumn id="15" xr3:uid="{42F79D9D-6A9A-4290-976D-8FC7D0C64550}" name="N.InVivoAUC" dataDxfId="5"/>
     <tableColumn id="9" xr3:uid="{26964959-0CEF-47FA-B3F1-3787B56AAF4B}" name="RMSLE.InVivoCmax" dataDxfId="4"/>
     <tableColumn id="7" xr3:uid="{C36A3E11-DF44-49AF-81EC-5DDE1C9E24BF}" name="N.InVivoCmax" dataDxfId="3"/>
-    <tableColumn id="18" xr3:uid="{DE399DF2-3D30-49D7-8319-CE0FA08C654A}" name="RMSLE.TissuePC" dataDxfId="0"/>
+    <tableColumn id="18" xr3:uid="{DE399DF2-3D30-49D7-8319-CE0FA08C654A}" name="RMSLE.TissuePC" dataDxfId="2"/>
     <tableColumn id="17" xr3:uid="{823AC9A4-09B8-47F3-A4C2-9EBE5D82251D}" name="N.TissuePC" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{77576EAB-F3B7-477C-9C89-32194666C30A}" name="Notes" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{77576EAB-F3B7-477C-9C89-32194666C30A}" name="Notes" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2980,10 +2998,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AA7C988-D5EA-4528-8554-7DA2671EBD43}">
-  <dimension ref="A1:R23"/>
+  <dimension ref="A1:R24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="R4" sqref="R4"/>
+    <sheetView tabSelected="1" topLeftCell="D4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="R24" sqref="R24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4249,6 +4267,62 @@
         <v>28</v>
       </c>
     </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A24" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B24" s="1">
+        <v>1023</v>
+      </c>
+      <c r="C24" s="1">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="D24" s="1">
+        <v>1</v>
+      </c>
+      <c r="E24" s="1">
+        <v>1</v>
+      </c>
+      <c r="F24" s="1">
+        <v>1.0629999999999999</v>
+      </c>
+      <c r="G24" s="1">
+        <v>352</v>
+      </c>
+      <c r="H24" s="1">
+        <v>0.29959999999999998</v>
+      </c>
+      <c r="I24" s="1">
+        <v>352</v>
+      </c>
+      <c r="J24" s="1">
+        <v>1.419</v>
+      </c>
+      <c r="K24" s="1">
+        <v>86</v>
+      </c>
+      <c r="L24" s="1">
+        <v>1.0469999999999999</v>
+      </c>
+      <c r="M24" s="1">
+        <v>86</v>
+      </c>
+      <c r="N24" s="1">
+        <v>1.33</v>
+      </c>
+      <c r="O24" s="1">
+        <v>86</v>
+      </c>
+      <c r="P24" s="1">
+        <v>0.63439999999999996</v>
+      </c>
+      <c r="Q24" s="1">
+        <v>863</v>
+      </c>
+      <c r="R24" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
Seems okay -- rat fabsgut broken
</commit_message>
<xml_diff>
--- a/datatables/httk-benchmarks.xlsx
+++ b/datatables/httk-benchmarks.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwambaug\git\httk-dev\datatables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF2A6746-B4AF-4CCF-96A2-50EBF81CE3B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D68E2F1-363D-4D6E-8FF7-6B4670B446C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{C208547E-DF7E-4D1E-AF51-B4A727438EC0}"/>
+    <workbookView xWindow="2160" yWindow="1830" windowWidth="16560" windowHeight="8970" xr2:uid="{C208547E-DF7E-4D1E-AF51-B4A727438EC0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>2.2.2</t>
   </si>
@@ -167,6 +167,12 @@
   </si>
   <si>
     <t>Used Caco-2 to replace Fabs=Fgut=1</t>
+  </si>
+  <si>
+    <t>2.3.1</t>
+  </si>
+  <si>
+    <t>Minor bug fixes</t>
   </si>
 </sst>
 </file>
@@ -389,9 +395,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$24</c:f>
+              <c:f>Sheet1!$A$2:$A$25</c:f>
               <c:strCache>
-                <c:ptCount val="23"/>
+                <c:ptCount val="24"/>
                 <c:pt idx="0">
                   <c:v>1.1</c:v>
                 </c:pt>
@@ -460,16 +466,19 @@
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>2.3.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2.3.1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$2:$F$24</c:f>
+              <c:f>Sheet1!$F$2:$F$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="23"/>
+                <c:ptCount val="24"/>
                 <c:pt idx="0">
                   <c:v>0.52929999999999999</c:v>
                 </c:pt>
@@ -538,6 +547,9 @@
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>1.0629999999999999</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.0109999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -976,9 +988,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$24</c:f>
+              <c:f>Sheet1!$A$2:$A$25</c:f>
               <c:strCache>
-                <c:ptCount val="23"/>
+                <c:ptCount val="24"/>
                 <c:pt idx="0">
                   <c:v>1.1</c:v>
                 </c:pt>
@@ -1047,16 +1059,19 @@
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>2.3.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2.3.1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$J$2:$J$24</c:f>
+              <c:f>Sheet1!$J$2:$J$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="23"/>
+                <c:ptCount val="24"/>
                 <c:pt idx="0">
                   <c:v>1.869</c:v>
                 </c:pt>
@@ -1125,6 +1140,9 @@
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>1.419</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.478</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2675,8 +2693,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3DD92D36-BFF3-413F-93A1-8D3D8569B858}" name="Table1" displayName="Table1" ref="A1:R24" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
-  <autoFilter ref="A1:R24" xr:uid="{3DD92D36-BFF3-413F-93A1-8D3D8569B858}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3DD92D36-BFF3-413F-93A1-8D3D8569B858}" name="Table1" displayName="Table1" ref="A1:R25" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
+  <autoFilter ref="A1:R25" xr:uid="{3DD92D36-BFF3-413F-93A1-8D3D8569B858}"/>
   <tableColumns count="18">
     <tableColumn id="1" xr3:uid="{478C9B49-D67B-44BA-B8BF-86E093E572FE}" name="Version" dataDxfId="17"/>
     <tableColumn id="13" xr3:uid="{1CCFB984-6FEC-43E4-BB73-000E230E2655}" name="N.steadystate" dataDxfId="16"/>
@@ -2998,10 +3016,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AA7C988-D5EA-4528-8554-7DA2671EBD43}">
-  <dimension ref="A1:R24"/>
+  <dimension ref="A1:R25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="R24" sqref="R24"/>
+    <sheetView tabSelected="1" topLeftCell="J19" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="R25" sqref="R25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4323,6 +4341,62 @@
         <v>42</v>
       </c>
     </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A25" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B25" s="1">
+        <v>1023</v>
+      </c>
+      <c r="C25" s="1">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="D25" s="1">
+        <v>1</v>
+      </c>
+      <c r="E25" s="1">
+        <v>1</v>
+      </c>
+      <c r="F25" s="1">
+        <v>1.0109999999999999</v>
+      </c>
+      <c r="G25" s="1">
+        <v>352</v>
+      </c>
+      <c r="H25" s="1">
+        <v>0.29049999999999998</v>
+      </c>
+      <c r="I25" s="1">
+        <v>352</v>
+      </c>
+      <c r="J25" s="1">
+        <v>1.478</v>
+      </c>
+      <c r="K25" s="1">
+        <v>29</v>
+      </c>
+      <c r="L25" s="1">
+        <v>1.1020000000000001</v>
+      </c>
+      <c r="M25" s="1">
+        <v>86</v>
+      </c>
+      <c r="N25" s="1">
+        <v>1.3759999999999999</v>
+      </c>
+      <c r="O25" s="1">
+        <v>86</v>
+      </c>
+      <c r="P25" s="1">
+        <v>0.63439999999999996</v>
+      </c>
+      <c r="Q25" s="1">
+        <v>863</v>
+      </c>
+      <c r="R25" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
Revert "Merge branch 'dev' into feature/fullterm_pregnancy"
This reverts commit 43f93fdef3097f54210896bd537cf59c82aca972, reversing
changes made to 29d9c56eb6cea171591e82d17e78ef7b3ca2c300.
</commit_message>
<xml_diff>
--- a/datatables/httk-benchmarks.xlsx
+++ b/datatables/httk-benchmarks.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwambaug\git\httk-dev\datatables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87ABACE5-AFBD-4793-8475-D3E6DD31383F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF2A6746-B4AF-4CCF-96A2-50EBF81CE3B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{C208547E-DF7E-4D1E-AF51-B4A727438EC0}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{C208547E-DF7E-4D1E-AF51-B4A727438EC0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>2.2.2</t>
   </si>
@@ -167,9 +167,6 @@
   </si>
   <si>
     <t>Used Caco-2 to replace Fabs=Fgut=1</t>
-  </si>
-  <si>
-    <t>2.3.1</t>
   </si>
 </sst>
 </file>
@@ -392,9 +389,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$25</c:f>
+              <c:f>Sheet1!$A$2:$A$24</c:f>
               <c:strCache>
-                <c:ptCount val="24"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>1.1</c:v>
                 </c:pt>
@@ -463,19 +460,16 @@
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>2.3.0</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>2.3.1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$2:$F$25</c:f>
+              <c:f>Sheet1!$F$2:$F$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="24"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>0.52929999999999999</c:v>
                 </c:pt>
@@ -544,9 +538,6 @@
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>1.0629999999999999</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>1.0109999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -985,9 +976,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$25</c:f>
+              <c:f>Sheet1!$A$2:$A$24</c:f>
               <c:strCache>
-                <c:ptCount val="24"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>1.1</c:v>
                 </c:pt>
@@ -1056,19 +1047,16 @@
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>2.3.0</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>2.3.1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$J$2:$J$25</c:f>
+              <c:f>Sheet1!$J$2:$J$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="24"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>1.869</c:v>
                 </c:pt>
@@ -1137,9 +1125,6 @@
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>1.419</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>1.478</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2690,8 +2675,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3DD92D36-BFF3-413F-93A1-8D3D8569B858}" name="Table1" displayName="Table1" ref="A1:R25" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
-  <autoFilter ref="A1:R25" xr:uid="{3DD92D36-BFF3-413F-93A1-8D3D8569B858}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3DD92D36-BFF3-413F-93A1-8D3D8569B858}" name="Table1" displayName="Table1" ref="A1:R24" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
+  <autoFilter ref="A1:R24" xr:uid="{3DD92D36-BFF3-413F-93A1-8D3D8569B858}"/>
   <tableColumns count="18">
     <tableColumn id="1" xr3:uid="{478C9B49-D67B-44BA-B8BF-86E093E572FE}" name="Version" dataDxfId="17"/>
     <tableColumn id="13" xr3:uid="{1CCFB984-6FEC-43E4-BB73-000E230E2655}" name="N.steadystate" dataDxfId="16"/>
@@ -3013,10 +2998,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AA7C988-D5EA-4528-8554-7DA2671EBD43}">
-  <dimension ref="A1:R25"/>
+  <dimension ref="A1:R24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" topLeftCell="D4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="R24" sqref="R24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4314,7 +4299,7 @@
         <v>1.419</v>
       </c>
       <c r="K24" s="1">
-        <v>29</v>
+        <v>86</v>
       </c>
       <c r="L24" s="1">
         <v>1.0469999999999999</v>
@@ -4337,60 +4322,6 @@
       <c r="R24" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A25" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B25" s="1">
-        <v>1023</v>
-      </c>
-      <c r="C25" s="1">
-        <v>0.99990000000000001</v>
-      </c>
-      <c r="D25" s="1">
-        <v>1</v>
-      </c>
-      <c r="E25" s="1">
-        <v>1</v>
-      </c>
-      <c r="F25" s="1">
-        <v>1.0109999999999999</v>
-      </c>
-      <c r="G25" s="1">
-        <v>352</v>
-      </c>
-      <c r="H25" s="1">
-        <v>0.29049999999999998</v>
-      </c>
-      <c r="I25" s="1">
-        <v>352</v>
-      </c>
-      <c r="J25" s="1">
-        <v>1.478</v>
-      </c>
-      <c r="K25" s="1">
-        <v>29</v>
-      </c>
-      <c r="L25" s="1">
-        <v>1.1020000000000001</v>
-      </c>
-      <c r="M25" s="1">
-        <v>86</v>
-      </c>
-      <c r="N25" s="1">
-        <v>1.3759999999999999</v>
-      </c>
-      <c r="O25" s="1">
-        <v>86</v>
-      </c>
-      <c r="P25" s="1">
-        <v>0.63439999999999996</v>
-      </c>
-      <c r="Q25" s="1">
-        <v>863</v>
-      </c>
-      <c r="R25" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Close to ready for CRAN
</commit_message>
<xml_diff>
--- a/datatables/httk-benchmarks.xlsx
+++ b/datatables/httk-benchmarks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwambaug\git\httk-dev\datatables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5160BAE-D46D-4CA9-8982-EF32D881593D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38BCB1C5-6EC2-401D-8E50-59E68CBD9959}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3930" yWindow="1080" windowWidth="14240" windowHeight="7810" xr2:uid="{C208547E-DF7E-4D1E-AF51-B4A727438EC0}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{C208547E-DF7E-4D1E-AF51-B4A727438EC0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>2.2.2</t>
   </si>
@@ -173,6 +173,9 @@
   </si>
   <si>
     <t>2.4.0</t>
+  </si>
+  <si>
+    <t>Switched to chem props from ctxR</t>
   </si>
 </sst>
 </file>
@@ -555,7 +558,7 @@
                   <c:v>1.0109999999999999</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.96479999999999999</c:v>
+                  <c:v>0.94769999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1154,7 +1157,7 @@
                   <c:v>1.478</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1.4319999999999999</c:v>
+                  <c:v>1.508</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3030,8 +3033,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AA7C988-D5EA-4528-8554-7DA2671EBD43}">
   <dimension ref="A1:R26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:XFD26"/>
+    <sheetView tabSelected="1" topLeftCell="D16" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4412,7 +4415,7 @@
         <v>44</v>
       </c>
       <c r="B26" s="1">
-        <v>1023</v>
+        <v>1021</v>
       </c>
       <c r="C26" s="1">
         <v>1</v>
@@ -4424,42 +4427,44 @@
         <v>1</v>
       </c>
       <c r="F26" s="1">
-        <v>0.96479999999999999</v>
+        <v>0.94769999999999999</v>
       </c>
       <c r="G26" s="1">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="H26" s="1">
-        <v>0.31359999999999999</v>
+        <v>0.27160000000000001</v>
       </c>
       <c r="I26" s="1">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="J26" s="1">
-        <v>1.4319999999999999</v>
+        <v>1.508</v>
       </c>
       <c r="K26" s="1">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="L26" s="1">
-        <v>1.3069999999999999</v>
+        <v>0.9698</v>
       </c>
       <c r="M26" s="1">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="N26" s="1">
-        <v>1.2989999999999999</v>
+        <v>1.1319999999999999</v>
       </c>
       <c r="O26" s="1">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="P26" s="1">
-        <v>0.63439999999999996</v>
+        <v>0.64659999999999995</v>
       </c>
       <c r="Q26" s="1">
         <v>863</v>
       </c>
-      <c r="R26" s="1"/>
+      <c r="R26" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Branched from CRAN release
</commit_message>
<xml_diff>
--- a/datatables/httk-benchmarks.xlsx
+++ b/datatables/httk-benchmarks.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwambaug\git\httk-dev\datatables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38BCB1C5-6EC2-401D-8E50-59E68CBD9959}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFEA8E62-ED29-4524-9209-2AC156417C5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{C208547E-DF7E-4D1E-AF51-B4A727438EC0}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>2.2.2</t>
   </si>
@@ -176,6 +176,12 @@
   </si>
   <si>
     <t>Switched to chem props from ctxR</t>
+  </si>
+  <si>
+    <t>2.5.0</t>
+  </si>
+  <si>
+    <t>Added models 3comp2 and sumclearances</t>
   </si>
 </sst>
 </file>
@@ -398,9 +404,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$26</c:f>
+              <c:f>Sheet1!$A$2:$A$27</c:f>
               <c:strCache>
-                <c:ptCount val="25"/>
+                <c:ptCount val="26"/>
                 <c:pt idx="0">
                   <c:v>1.1</c:v>
                 </c:pt>
@@ -475,16 +481,19 @@
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>2.4.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2.5.0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$2:$F$26</c:f>
+              <c:f>Sheet1!$F$2:$F$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="25"/>
+                <c:ptCount val="26"/>
                 <c:pt idx="0">
                   <c:v>0.52929999999999999</c:v>
                 </c:pt>
@@ -558,6 +567,9 @@
                   <c:v>1.0109999999999999</c:v>
                 </c:pt>
                 <c:pt idx="24">
+                  <c:v>0.94769999999999999</c:v>
+                </c:pt>
+                <c:pt idx="25">
                   <c:v>0.94769999999999999</c:v>
                 </c:pt>
               </c:numCache>
@@ -997,9 +1009,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$26</c:f>
+              <c:f>Sheet1!$A$2:$A$27</c:f>
               <c:strCache>
-                <c:ptCount val="25"/>
+                <c:ptCount val="26"/>
                 <c:pt idx="0">
                   <c:v>1.1</c:v>
                 </c:pt>
@@ -1074,16 +1086,19 @@
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>2.4.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2.5.0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$J$2:$J$26</c:f>
+              <c:f>Sheet1!$J$2:$J$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="25"/>
+                <c:ptCount val="26"/>
                 <c:pt idx="0">
                   <c:v>1.869</c:v>
                 </c:pt>
@@ -1157,6 +1172,9 @@
                   <c:v>1.478</c:v>
                 </c:pt>
                 <c:pt idx="24">
+                  <c:v>1.508</c:v>
+                </c:pt>
+                <c:pt idx="25">
                   <c:v>1.508</c:v>
                 </c:pt>
               </c:numCache>
@@ -2708,8 +2726,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3DD92D36-BFF3-413F-93A1-8D3D8569B858}" name="Table1" displayName="Table1" ref="A1:R26" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
-  <autoFilter ref="A1:R26" xr:uid="{3DD92D36-BFF3-413F-93A1-8D3D8569B858}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3DD92D36-BFF3-413F-93A1-8D3D8569B858}" name="Table1" displayName="Table1" ref="A1:R27" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
+  <autoFilter ref="A1:R27" xr:uid="{3DD92D36-BFF3-413F-93A1-8D3D8569B858}"/>
   <tableColumns count="18">
     <tableColumn id="1" xr3:uid="{478C9B49-D67B-44BA-B8BF-86E093E572FE}" name="Version" dataDxfId="17"/>
     <tableColumn id="13" xr3:uid="{1CCFB984-6FEC-43E4-BB73-000E230E2655}" name="N.steadystate" dataDxfId="16"/>
@@ -2735,9 +2753,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2775,7 +2793,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2881,7 +2899,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3023,7 +3041,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3031,10 +3049,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AA7C988-D5EA-4528-8554-7DA2671EBD43}">
-  <dimension ref="A1:R26"/>
+  <dimension ref="A1:R27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D16" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" topLeftCell="I16" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="R27" sqref="R27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4466,6 +4484,62 @@
         <v>45</v>
       </c>
     </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A27" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B27" s="1">
+        <v>1021</v>
+      </c>
+      <c r="C27" s="1">
+        <v>1</v>
+      </c>
+      <c r="D27" s="1">
+        <v>1</v>
+      </c>
+      <c r="E27" s="1">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="F27" s="1">
+        <v>0.94769999999999999</v>
+      </c>
+      <c r="G27" s="1">
+        <v>353</v>
+      </c>
+      <c r="H27" s="1">
+        <v>0.27160000000000001</v>
+      </c>
+      <c r="I27" s="1">
+        <v>353</v>
+      </c>
+      <c r="J27" s="1">
+        <v>1.508</v>
+      </c>
+      <c r="K27" s="1">
+        <v>36</v>
+      </c>
+      <c r="L27" s="1">
+        <v>0.9698</v>
+      </c>
+      <c r="M27" s="1">
+        <v>80</v>
+      </c>
+      <c r="N27" s="1">
+        <v>1.1319999999999999</v>
+      </c>
+      <c r="O27" s="1">
+        <v>80</v>
+      </c>
+      <c r="P27" s="1">
+        <v>0.64659999999999995</v>
+      </c>
+      <c r="Q27" s="1">
+        <v>863</v>
+      </c>
+      <c r="R27" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
We want data tables from dev
</commit_message>
<xml_diff>
--- a/datatables/httk-benchmarks.xlsx
+++ b/datatables/httk-benchmarks.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwambaug\git\httk-dev\datatables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38BCB1C5-6EC2-401D-8E50-59E68CBD9959}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFEA8E62-ED29-4524-9209-2AC156417C5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{C208547E-DF7E-4D1E-AF51-B4A727438EC0}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>2.2.2</t>
   </si>
@@ -176,6 +176,12 @@
   </si>
   <si>
     <t>Switched to chem props from ctxR</t>
+  </si>
+  <si>
+    <t>2.5.0</t>
+  </si>
+  <si>
+    <t>Added models 3comp2 and sumclearances</t>
   </si>
 </sst>
 </file>
@@ -398,9 +404,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$26</c:f>
+              <c:f>Sheet1!$A$2:$A$27</c:f>
               <c:strCache>
-                <c:ptCount val="25"/>
+                <c:ptCount val="26"/>
                 <c:pt idx="0">
                   <c:v>1.1</c:v>
                 </c:pt>
@@ -475,16 +481,19 @@
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>2.4.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2.5.0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$2:$F$26</c:f>
+              <c:f>Sheet1!$F$2:$F$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="25"/>
+                <c:ptCount val="26"/>
                 <c:pt idx="0">
                   <c:v>0.52929999999999999</c:v>
                 </c:pt>
@@ -558,6 +567,9 @@
                   <c:v>1.0109999999999999</c:v>
                 </c:pt>
                 <c:pt idx="24">
+                  <c:v>0.94769999999999999</c:v>
+                </c:pt>
+                <c:pt idx="25">
                   <c:v>0.94769999999999999</c:v>
                 </c:pt>
               </c:numCache>
@@ -997,9 +1009,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$26</c:f>
+              <c:f>Sheet1!$A$2:$A$27</c:f>
               <c:strCache>
-                <c:ptCount val="25"/>
+                <c:ptCount val="26"/>
                 <c:pt idx="0">
                   <c:v>1.1</c:v>
                 </c:pt>
@@ -1074,16 +1086,19 @@
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>2.4.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2.5.0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$J$2:$J$26</c:f>
+              <c:f>Sheet1!$J$2:$J$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="25"/>
+                <c:ptCount val="26"/>
                 <c:pt idx="0">
                   <c:v>1.869</c:v>
                 </c:pt>
@@ -1157,6 +1172,9 @@
                   <c:v>1.478</c:v>
                 </c:pt>
                 <c:pt idx="24">
+                  <c:v>1.508</c:v>
+                </c:pt>
+                <c:pt idx="25">
                   <c:v>1.508</c:v>
                 </c:pt>
               </c:numCache>
@@ -2708,8 +2726,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3DD92D36-BFF3-413F-93A1-8D3D8569B858}" name="Table1" displayName="Table1" ref="A1:R26" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
-  <autoFilter ref="A1:R26" xr:uid="{3DD92D36-BFF3-413F-93A1-8D3D8569B858}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3DD92D36-BFF3-413F-93A1-8D3D8569B858}" name="Table1" displayName="Table1" ref="A1:R27" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
+  <autoFilter ref="A1:R27" xr:uid="{3DD92D36-BFF3-413F-93A1-8D3D8569B858}"/>
   <tableColumns count="18">
     <tableColumn id="1" xr3:uid="{478C9B49-D67B-44BA-B8BF-86E093E572FE}" name="Version" dataDxfId="17"/>
     <tableColumn id="13" xr3:uid="{1CCFB984-6FEC-43E4-BB73-000E230E2655}" name="N.steadystate" dataDxfId="16"/>
@@ -2735,9 +2753,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2775,7 +2793,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2881,7 +2899,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3023,7 +3041,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3031,10 +3049,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AA7C988-D5EA-4528-8554-7DA2671EBD43}">
-  <dimension ref="A1:R26"/>
+  <dimension ref="A1:R27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D16" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" topLeftCell="I16" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="R27" sqref="R27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4466,6 +4484,62 @@
         <v>45</v>
       </c>
     </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A27" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B27" s="1">
+        <v>1021</v>
+      </c>
+      <c r="C27" s="1">
+        <v>1</v>
+      </c>
+      <c r="D27" s="1">
+        <v>1</v>
+      </c>
+      <c r="E27" s="1">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="F27" s="1">
+        <v>0.94769999999999999</v>
+      </c>
+      <c r="G27" s="1">
+        <v>353</v>
+      </c>
+      <c r="H27" s="1">
+        <v>0.27160000000000001</v>
+      </c>
+      <c r="I27" s="1">
+        <v>353</v>
+      </c>
+      <c r="J27" s="1">
+        <v>1.508</v>
+      </c>
+      <c r="K27" s="1">
+        <v>36</v>
+      </c>
+      <c r="L27" s="1">
+        <v>0.9698</v>
+      </c>
+      <c r="M27" s="1">
+        <v>80</v>
+      </c>
+      <c r="N27" s="1">
+        <v>1.1319999999999999</v>
+      </c>
+      <c r="O27" s="1">
+        <v>80</v>
+      </c>
+      <c r="P27" s="1">
+        <v>0.64659999999999995</v>
+      </c>
+      <c r="Q27" s="1">
+        <v>863</v>
+      </c>
+      <c r="R27" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
bugs caught by R CMD check
</commit_message>
<xml_diff>
--- a/datatables/httk-benchmarks.xlsx
+++ b/datatables/httk-benchmarks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwambaug\git\httk-dev\datatables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0204AE81-40EB-472A-84F2-B7903430204C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{852508E6-3090-4F08-89CC-2015F37FAB3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{C208547E-DF7E-4D1E-AF51-B4A727438EC0}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>2.2.2</t>
   </si>
@@ -188,6 +188,9 @@
   </si>
   <si>
     <t>Added first trimester model</t>
+  </si>
+  <si>
+    <t>2.6.1</t>
   </si>
 </sst>
 </file>
@@ -410,9 +413,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$28</c:f>
+              <c:f>Sheet1!$A$2:$A$29</c:f>
               <c:strCache>
-                <c:ptCount val="27"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
                   <c:v>1.1</c:v>
                 </c:pt>
@@ -493,16 +496,19 @@
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>2.6.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2.6.1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$2:$F$28</c:f>
+              <c:f>Sheet1!$F$2:$F$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
                   <c:v>0.52929999999999999</c:v>
                 </c:pt>
@@ -1021,9 +1027,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$28</c:f>
+              <c:f>Sheet1!$A$2:$A$29</c:f>
               <c:strCache>
-                <c:ptCount val="27"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
                   <c:v>1.1</c:v>
                 </c:pt>
@@ -1104,16 +1110,19 @@
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>2.6.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2.6.1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$J$2:$J$28</c:f>
+              <c:f>Sheet1!$J$2:$J$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
                   <c:v>1.869</c:v>
                 </c:pt>
@@ -2744,8 +2753,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3DD92D36-BFF3-413F-93A1-8D3D8569B858}" name="Table1" displayName="Table1" ref="A1:R28" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
-  <autoFilter ref="A1:R28" xr:uid="{3DD92D36-BFF3-413F-93A1-8D3D8569B858}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3DD92D36-BFF3-413F-93A1-8D3D8569B858}" name="Table1" displayName="Table1" ref="A1:R29" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
+  <autoFilter ref="A1:R29" xr:uid="{3DD92D36-BFF3-413F-93A1-8D3D8569B858}"/>
   <tableColumns count="18">
     <tableColumn id="1" xr3:uid="{478C9B49-D67B-44BA-B8BF-86E093E572FE}" name="Version" dataDxfId="17"/>
     <tableColumn id="13" xr3:uid="{1CCFB984-6FEC-43E4-BB73-000E230E2655}" name="N.steadystate" dataDxfId="16"/>
@@ -3067,10 +3076,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AA7C988-D5EA-4528-8554-7DA2671EBD43}">
-  <dimension ref="A1:R28"/>
+  <dimension ref="A1:R29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I16" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="R28" sqref="R28"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4614,6 +4623,36 @@
         <v>49</v>
       </c>
     </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A29" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B29" s="1">
+        <v>1007</v>
+      </c>
+      <c r="C29" s="1">
+        <v>0.99980000000000002</v>
+      </c>
+      <c r="D29" s="1">
+        <v>1</v>
+      </c>
+      <c r="E29" s="1">
+        <v>1.0009999999999999</v>
+      </c>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
+      <c r="L29" s="1"/>
+      <c r="M29" s="1"/>
+      <c r="N29" s="1"/>
+      <c r="O29" s="1"/>
+      <c r="P29" s="1"/>
+      <c r="Q29" s="1"/>
+      <c r="R29" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
Add missing physchem, properly read Lynn data, solve CRAN test issue
</commit_message>
<xml_diff>
--- a/datatables/httk-benchmarks.xlsx
+++ b/datatables/httk-benchmarks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwambaug\git\httk-dev\datatables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{852508E6-3090-4F08-89CC-2015F37FAB3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47B7FEEE-59B3-4114-A698-2FA559D9BC33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{C208547E-DF7E-4D1E-AF51-B4A727438EC0}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t>2.2.2</t>
   </si>
@@ -191,6 +191,9 @@
   </si>
   <si>
     <t>2.6.1</t>
+  </si>
+  <si>
+    <t>Updated pKa's with ChemAxon</t>
   </si>
 </sst>
 </file>
@@ -589,6 +592,9 @@
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>0.94769999999999999</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.9325</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1204,6 +1210,9 @@
                 <c:pt idx="26">
                   <c:v>1.508</c:v>
                 </c:pt>
+                <c:pt idx="27">
+                  <c:v>1.7350000000000001</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3078,8 +3087,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AA7C988-D5EA-4528-8554-7DA2671EBD43}">
   <dimension ref="A1:R29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="C17" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="M29" sqref="M29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4628,7 +4637,7 @@
         <v>50</v>
       </c>
       <c r="B29" s="1">
-        <v>1007</v>
+        <v>1026</v>
       </c>
       <c r="C29" s="1">
         <v>0.99980000000000002</v>
@@ -4639,19 +4648,45 @@
       <c r="E29" s="1">
         <v>1.0009999999999999</v>
       </c>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
-      <c r="J29" s="1"/>
-      <c r="K29" s="1"/>
-      <c r="L29" s="1"/>
-      <c r="M29" s="1"/>
-      <c r="N29" s="1"/>
-      <c r="O29" s="1"/>
-      <c r="P29" s="1"/>
-      <c r="Q29" s="1"/>
-      <c r="R29" s="1"/>
+      <c r="F29" s="1">
+        <v>0.9325</v>
+      </c>
+      <c r="G29" s="1">
+        <v>353</v>
+      </c>
+      <c r="H29" s="1">
+        <v>0.2296</v>
+      </c>
+      <c r="I29" s="1">
+        <v>353</v>
+      </c>
+      <c r="J29" s="1">
+        <v>1.7350000000000001</v>
+      </c>
+      <c r="K29" s="1">
+        <v>36</v>
+      </c>
+      <c r="L29" s="1">
+        <v>1.143</v>
+      </c>
+      <c r="M29" s="1">
+        <v>80</v>
+      </c>
+      <c r="N29" s="1">
+        <v>1.2390000000000001</v>
+      </c>
+      <c r="O29" s="1">
+        <v>80</v>
+      </c>
+      <c r="P29" s="1">
+        <v>0.60919999999999996</v>
+      </c>
+      <c r="Q29" s="1">
+        <v>863</v>
+      </c>
+      <c r="R29" s="1" t="s">
+        <v>51</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
initial submission to CRAN
</commit_message>
<xml_diff>
--- a/datatables/httk-benchmarks.xlsx
+++ b/datatables/httk-benchmarks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwambaug\git\httk-dev\datatables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47B7FEEE-59B3-4114-A698-2FA559D9BC33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B75FE65-5D4B-4B16-A6CA-C39FBCC7BFEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{C208547E-DF7E-4D1E-AF51-B4A727438EC0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{C208547E-DF7E-4D1E-AF51-B4A727438EC0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>2.2.2</t>
   </si>
@@ -194,6 +194,12 @@
   </si>
   <si>
     <t>Updated pKa's with ChemAxon</t>
+  </si>
+  <si>
+    <t>2.7.0</t>
+  </si>
+  <si>
+    <t>Updated CvT data, added pfas, dermal models, updated IVD models</t>
   </si>
 </sst>
 </file>
@@ -416,9 +422,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$29</c:f>
+              <c:f>Sheet1!$A$2:$A$30</c:f>
               <c:strCache>
-                <c:ptCount val="28"/>
+                <c:ptCount val="29"/>
                 <c:pt idx="0">
                   <c:v>1.1</c:v>
                 </c:pt>
@@ -502,16 +508,19 @@
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>2.6.1</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2.7.0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$2:$F$29</c:f>
+              <c:f>Sheet1!$F$2:$F$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="28"/>
+                <c:ptCount val="29"/>
                 <c:pt idx="0">
                   <c:v>0.52929999999999999</c:v>
                 </c:pt>
@@ -595,6 +604,9 @@
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>0.9325</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.93500000000000005</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1033,9 +1045,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$29</c:f>
+              <c:f>Sheet1!$A$2:$A$30</c:f>
               <c:strCache>
-                <c:ptCount val="28"/>
+                <c:ptCount val="29"/>
                 <c:pt idx="0">
                   <c:v>1.1</c:v>
                 </c:pt>
@@ -1119,16 +1131,19 @@
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>2.6.1</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2.7.0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$J$2:$J$29</c:f>
+              <c:f>Sheet1!$J$2:$J$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="28"/>
+                <c:ptCount val="29"/>
                 <c:pt idx="0">
                   <c:v>1.869</c:v>
                 </c:pt>
@@ -1212,6 +1227,9 @@
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>1.7350000000000001</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2.3740000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2762,8 +2780,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3DD92D36-BFF3-413F-93A1-8D3D8569B858}" name="Table1" displayName="Table1" ref="A1:R29" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
-  <autoFilter ref="A1:R29" xr:uid="{3DD92D36-BFF3-413F-93A1-8D3D8569B858}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3DD92D36-BFF3-413F-93A1-8D3D8569B858}" name="Table1" displayName="Table1" ref="A1:R30" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
+  <autoFilter ref="A1:R30" xr:uid="{3DD92D36-BFF3-413F-93A1-8D3D8569B858}"/>
   <tableColumns count="18">
     <tableColumn id="1" xr3:uid="{478C9B49-D67B-44BA-B8BF-86E093E572FE}" name="Version" dataDxfId="17"/>
     <tableColumn id="13" xr3:uid="{1CCFB984-6FEC-43E4-BB73-000E230E2655}" name="N.steadystate" dataDxfId="16"/>
@@ -3085,24 +3103,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AA7C988-D5EA-4528-8554-7DA2671EBD43}">
-  <dimension ref="A1:R29"/>
+  <dimension ref="A1:R30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C17" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="M29" sqref="M29"/>
+    <sheetView tabSelected="1" topLeftCell="C10" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="5" width="10.36328125" customWidth="1"/>
-    <col min="6" max="6" width="16.90625" customWidth="1"/>
-    <col min="7" max="7" width="12.81640625" customWidth="1"/>
-    <col min="8" max="8" width="13.81640625" customWidth="1"/>
-    <col min="9" max="10" width="9.7265625" customWidth="1"/>
-    <col min="11" max="17" width="6.7265625" customWidth="1"/>
-    <col min="18" max="18" width="39.453125" customWidth="1"/>
+    <col min="1" max="5" width="10.42578125" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" customWidth="1"/>
+    <col min="9" max="10" width="9.7109375" customWidth="1"/>
+    <col min="11" max="17" width="6.7109375" customWidth="1"/>
+    <col min="18" max="18" width="39.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -3158,7 +3176,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1.1000000000000001</v>
       </c>
@@ -3208,7 +3226,7 @@
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1.2</v>
       </c>
@@ -3258,7 +3276,7 @@
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1.3</v>
       </c>
@@ -3312,7 +3330,7 @@
       </c>
       <c r="R4" s="1"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>1.4</v>
       </c>
@@ -3366,7 +3384,7 @@
       </c>
       <c r="R5" s="1"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>1.5</v>
       </c>
@@ -3422,7 +3440,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>1.6</v>
       </c>
@@ -3478,7 +3496,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>1.7</v>
       </c>
@@ -3532,7 +3550,7 @@
       </c>
       <c r="R8" s="1"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>1.8</v>
       </c>
@@ -3586,7 +3604,7 @@
       </c>
       <c r="R9" s="1"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>1.9</v>
       </c>
@@ -3640,7 +3658,7 @@
       </c>
       <c r="R10" s="1"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
@@ -3696,7 +3714,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>4</v>
       </c>
@@ -3750,7 +3768,7 @@
       </c>
       <c r="R12" s="1"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
@@ -3806,7 +3824,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>17</v>
       </c>
@@ -3860,7 +3878,7 @@
       </c>
       <c r="R14" s="1"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>7</v>
       </c>
@@ -3916,7 +3934,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -3970,7 +3988,7 @@
       </c>
       <c r="R16" s="1"/>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>13</v>
       </c>
@@ -4024,7 +4042,7 @@
       </c>
       <c r="R17" s="1"/>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>12</v>
       </c>
@@ -4078,7 +4096,7 @@
       </c>
       <c r="R18" s="1"/>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>11</v>
       </c>
@@ -4132,7 +4150,7 @@
       </c>
       <c r="R19" s="1"/>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>10</v>
       </c>
@@ -4188,7 +4206,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>9</v>
       </c>
@@ -4244,7 +4262,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>3</v>
       </c>
@@ -4298,7 +4316,7 @@
       </c>
       <c r="R22" s="1"/>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>0</v>
       </c>
@@ -4354,7 +4372,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>41</v>
       </c>
@@ -4410,7 +4428,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>43</v>
       </c>
@@ -4464,7 +4482,7 @@
       </c>
       <c r="R25" s="1"/>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>44</v>
       </c>
@@ -4520,7 +4538,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>46</v>
       </c>
@@ -4576,7 +4594,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>48</v>
       </c>
@@ -4632,7 +4650,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>50</v>
       </c>
@@ -4686,6 +4704,62 @@
       </c>
       <c r="R29" s="1" t="s">
         <v>51</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B30" s="1">
+        <v>1026</v>
+      </c>
+      <c r="C30" s="1">
+        <v>0.99980000000000002</v>
+      </c>
+      <c r="D30" s="1">
+        <v>1</v>
+      </c>
+      <c r="E30" s="1">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="F30" s="1">
+        <v>0.93500000000000005</v>
+      </c>
+      <c r="G30" s="1">
+        <v>352</v>
+      </c>
+      <c r="H30" s="1">
+        <v>0.2712</v>
+      </c>
+      <c r="I30" s="1">
+        <v>352</v>
+      </c>
+      <c r="J30" s="1">
+        <v>2.3740000000000001</v>
+      </c>
+      <c r="K30" s="1">
+        <v>43</v>
+      </c>
+      <c r="L30" s="1">
+        <v>1.5309999999999999</v>
+      </c>
+      <c r="M30" s="1">
+        <v>160</v>
+      </c>
+      <c r="N30" s="1">
+        <v>1.202</v>
+      </c>
+      <c r="O30" s="1">
+        <v>160</v>
+      </c>
+      <c r="P30" s="1">
+        <v>0.629</v>
+      </c>
+      <c r="Q30" s="1">
+        <v>863</v>
+      </c>
+      <c r="R30" s="1" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
benchmark httk working with new pk fits
</commit_message>
<xml_diff>
--- a/datatables/httk-benchmarks.xlsx
+++ b/datatables/httk-benchmarks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwambaug\git\httk-dev\datatables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B75FE65-5D4B-4B16-A6CA-C39FBCC7BFEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12ECD942-4BD4-4BA7-98E4-39DD13801945}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{C208547E-DF7E-4D1E-AF51-B4A727438EC0}"/>
+    <workbookView xWindow="1215" yWindow="1365" windowWidth="27585" windowHeight="11820" xr2:uid="{C208547E-DF7E-4D1E-AF51-B4A727438EC0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
   <si>
     <t>2.2.2</t>
   </si>
@@ -200,6 +200,12 @@
   </si>
   <si>
     <t>Updated CvT data, added pfas, dermal models, updated IVD models</t>
+  </si>
+  <si>
+    <t>2.7.1</t>
+  </si>
+  <si>
+    <t>Updated CvTdb fits (invivoPKfit)</t>
   </si>
 </sst>
 </file>
@@ -422,9 +428,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$30</c:f>
+              <c:f>Sheet1!$A$2:$A$31</c:f>
               <c:strCache>
-                <c:ptCount val="29"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
                   <c:v>1.1</c:v>
                 </c:pt>
@@ -511,16 +517,19 @@
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>2.7.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2.7.1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$2:$F$30</c:f>
+              <c:f>Sheet1!$F$2:$F$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="29"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
                   <c:v>0.52929999999999999</c:v>
                 </c:pt>
@@ -606,6 +615,9 @@
                   <c:v>0.9325</c:v>
                 </c:pt>
                 <c:pt idx="28">
+                  <c:v>0.93500000000000005</c:v>
+                </c:pt>
+                <c:pt idx="29">
                   <c:v>0.93500000000000005</c:v>
                 </c:pt>
               </c:numCache>
@@ -1045,9 +1057,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$30</c:f>
+              <c:f>Sheet1!$A$2:$A$31</c:f>
               <c:strCache>
-                <c:ptCount val="29"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
                   <c:v>1.1</c:v>
                 </c:pt>
@@ -1134,16 +1146,19 @@
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>2.7.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2.7.1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$J$2:$J$30</c:f>
+              <c:f>Sheet1!$J$2:$J$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="29"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
                   <c:v>1.869</c:v>
                 </c:pt>
@@ -1230,6 +1245,9 @@
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>2.3740000000000001</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2.1840000000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2780,8 +2798,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3DD92D36-BFF3-413F-93A1-8D3D8569B858}" name="Table1" displayName="Table1" ref="A1:R30" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
-  <autoFilter ref="A1:R30" xr:uid="{3DD92D36-BFF3-413F-93A1-8D3D8569B858}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3DD92D36-BFF3-413F-93A1-8D3D8569B858}" name="Table1" displayName="Table1" ref="A1:R31" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
+  <autoFilter ref="A1:R31" xr:uid="{3DD92D36-BFF3-413F-93A1-8D3D8569B858}"/>
   <tableColumns count="18">
     <tableColumn id="1" xr3:uid="{478C9B49-D67B-44BA-B8BF-86E093E572FE}" name="Version" dataDxfId="17"/>
     <tableColumn id="13" xr3:uid="{1CCFB984-6FEC-43E4-BB73-000E230E2655}" name="N.steadystate" dataDxfId="16"/>
@@ -3103,10 +3121,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AA7C988-D5EA-4528-8554-7DA2671EBD43}">
-  <dimension ref="A1:R30"/>
+  <dimension ref="A1:R31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C10" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="J30" sqref="J30"/>
+    <sheetView tabSelected="1" topLeftCell="G22" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4762,6 +4780,62 @@
         <v>53</v>
       </c>
     </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B31" s="1">
+        <v>1026</v>
+      </c>
+      <c r="C31" s="1">
+        <v>0.99980000000000002</v>
+      </c>
+      <c r="D31" s="1">
+        <v>1</v>
+      </c>
+      <c r="E31" s="1">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="F31" s="1">
+        <v>0.93500000000000005</v>
+      </c>
+      <c r="G31" s="1">
+        <v>352</v>
+      </c>
+      <c r="H31" s="1">
+        <v>0.2712</v>
+      </c>
+      <c r="I31" s="1">
+        <v>352</v>
+      </c>
+      <c r="J31" s="1">
+        <v>2.1840000000000002</v>
+      </c>
+      <c r="K31" s="1">
+        <v>100</v>
+      </c>
+      <c r="L31" s="1">
+        <v>1.2929999999999999</v>
+      </c>
+      <c r="M31" s="1">
+        <v>112</v>
+      </c>
+      <c r="N31" s="1">
+        <v>1.2130000000000001</v>
+      </c>
+      <c r="O31" s="1">
+        <v>156</v>
+      </c>
+      <c r="P31" s="1">
+        <v>0.26290000000000002</v>
+      </c>
+      <c r="Q31" s="1">
+        <v>863</v>
+      </c>
+      <c r="R31" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>